<commit_message>
clean up and edits
Cleaned redundant files used during testing.

Changed resoning prompt and made mode to be max value in case of dispute.
</commit_message>
<xml_diff>
--- a/approach2_exp/results/jdk_1.xlsx
+++ b/approach2_exp/results/jdk_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>project_count</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>reason</t>
         </is>
       </c>
@@ -458,11 +463,15 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>76.76000000000001</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> The candidate has strong technical skills, experience and knowledge in MERN Stack, ReactJS, Django, Python, JavaScript and Computer Vision, Image Processing. The projects they have worked on demonstrate their competency and the score of 76.76 reflects this.</t>
+        <v>73.92</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+The candidate has a score of 73.92 as they have experience in the relevant technologies required for the job, such as MongoDB, ReactJS, JavaScript, Web Development, NodeJS, as well as other related technologies such as Python, Django, Computer Vision, Image Processing. Their projects demonstrate their ability to work on developing web/mobile applications, feature development, scalability, and product enhancement.</t>
         </is>
       </c>
     </row>
@@ -474,12 +483,15 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>91.87</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-The candidate has the perfect blend of technical skills and project experience to fill the role of SDE Intern. They have used the mentioned technologies in their projects and have demonstrated the ability to develop quality web/mobile applications. Their score of 91.87 reflects their aptitude for this role.</t>
+        <v>90.47</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 
+Reasoning: The candidate has demonstrated strong expertise in technologies relevant to the job description, such as MongoDB, ReactJS, JavaScript, Web Development, NodeJS, HTML, CSS, Socket.IO, WebRTC, Flutter, Dart, Firebase. Their projects also showcase a good understanding of the technologies and how to use them in combination to develop web/mobile applications. The candidate's score reflects their ability to develop high-quality applications in the aforementioned technologies.</t>
         </is>
       </c>
     </row>
@@ -491,11 +503,15 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>80.26000000000001</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> The applicant has a strong background in MERN Stack, Django Rest Framework, ReactJS, PyTorch, Tensorflow, Keras, and Sklearn, which are essential skills for the SDE Intern role. The candidate has experience with building websites, post-processing of large language models, and multi-model data analysis for annotation of human activities, demonstrating their aptness for the job and resulting in a score of 80.26.</t>
+        <v>78.58</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Reasoning: The candidate has demonstrated technical proficiency in MongoDB, ReactJS, JavaScript, Web Development, NodeJS, Django Rest Framework, Pytorch, Tensorflow, Keras, and Sklearn, which are the skills required for the job. The projects showcase the candidate's ability to design and develop high-quality web/mobile applications, integrate machine learning models with user interfaces, and develop automated pipelines for multi-model data analysis. All these qualities make the candidate a good fit for the job, justifying their score of 78.58.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changed file name for candidate scoring
Initial Name: embed_query
Current: hrassistant

Also changed prompts a bit.
</commit_message>
<xml_diff>
--- a/approach2_exp/results/jdk_1.xlsx
+++ b/approach2_exp/results/jdk_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,10 +460,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>73.92</v>
+        <v>85.48</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -471,7 +471,7 @@
       <c r="E2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-The candidate has a score of 73.92 as they have experience in the relevant technologies required for the job, such as MongoDB, ReactJS, JavaScript, Web Development, NodeJS, as well as other related technologies such as Python, Django, Computer Vision, Image Processing. Their projects demonstrate their ability to work on developing web/mobile applications, feature development, scalability, and product enhancement.</t>
+Reasoning: The candidate has a strong skillset related to the job description, having worked with the MERN stack, ReactJS, NodeJS, ExpressJS, Socket.IO, WebRTC, HTML, CSS, and JS. The projects they have worked on demonstrate their ability to create and design web/mobile applications, manage data, and develop features with scalability. The score of 85.48 reflects their aptitude for the job.</t>
         </is>
       </c>
     </row>
@@ -480,38 +480,18 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>90.47</v>
+        <v>74.48</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 
-Reasoning: The candidate has demonstrated strong expertise in technologies relevant to the job description, such as MongoDB, ReactJS, JavaScript, Web Development, NodeJS, HTML, CSS, Socket.IO, WebRTC, Flutter, Dart, Firebase. Their projects also showcase a good understanding of the technologies and how to use them in combination to develop web/mobile applications. The candidate's score reflects their ability to develop high-quality applications in the aforementioned technologies.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="n">
-        <v>78.58</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
           <t xml:space="preserve">
-Reasoning: The candidate has demonstrated technical proficiency in MongoDB, ReactJS, JavaScript, Web Development, NodeJS, Django Rest Framework, Pytorch, Tensorflow, Keras, and Sklearn, which are the skills required for the job. The projects showcase the candidate's ability to design and develop high-quality web/mobile applications, integrate machine learning models with user interfaces, and develop automated pipelines for multi-model data analysis. All these qualities make the candidate a good fit for the job, justifying their score of 78.58.</t>
+Reasoning: The candidate has demonstrated excellent technical skills and knowledge of the MERN stack, Django Rest Framework, Pytorch, Tensorflow, Keras, and Sklearn. He has also shown experience in developing web/mobile applications, library management systems, user interfaces, and machine learning models. With these skills, he is well suited for the job and has been given a score of 74.48.</t>
         </is>
       </c>
     </row>

</xml_diff>